<commit_message>
fix repors and add missing diagrams
</commit_message>
<xml_diff>
--- a/reports/Results.xlsx
+++ b/reports/Results.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10609"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10811"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/moe/Desktop/puf-auth-ml/reports/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{14526427-1DD8-454D-9E1E-C3672CAA7A43}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4D71D96B-3BB4-FD46-9745-56A07A170188}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="500" windowWidth="28800" windowHeight="16120" xr2:uid="{65BD7D84-E0D3-BF4C-8AA6-282CCD8082D7}"/>
+    <workbookView xWindow="4160" yWindow="4280" windowWidth="28800" windowHeight="16120" xr2:uid="{65BD7D84-E0D3-BF4C-8AA6-282CCD8082D7}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="302" uniqueCount="171">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="302" uniqueCount="174">
   <si>
     <t>Intact</t>
   </si>
@@ -372,9 +372,6 @@
   </si>
   <si>
     <t>94.81%</t>
-  </si>
-  <si>
-    <t>77.27%</t>
   </si>
   <si>
     <t>93.55%</t>
@@ -1112,6 +1109,18 @@
   </si>
   <si>
     <t>87% Confidence to Unknown</t>
+  </si>
+  <si>
+    <t>77.26%</t>
+  </si>
+  <si>
+    <t>90.99%</t>
+  </si>
+  <si>
+    <t>89.52%</t>
+  </si>
+  <si>
+    <t>66.41%</t>
   </si>
 </sst>
 </file>
@@ -1374,7 +1383,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="74">
+  <cellXfs count="73">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
@@ -1520,44 +1529,13 @@
     </xf>
     <xf numFmtId="0" fontId="2" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="right"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="3" fillId="2" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -1566,6 +1544,36 @@
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -2317,8 +2325,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1F7AB769-A4AB-314C-9FAA-CEF8525B9786}">
   <dimension ref="F6:V104"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="I57" zoomScaleNormal="88" workbookViewId="0">
-      <selection activeCell="O72" sqref="O72"/>
+    <sheetView tabSelected="1" topLeftCell="N31" zoomScaleNormal="88" workbookViewId="0">
+      <selection activeCell="T43" sqref="T43"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -2340,50 +2348,50 @@
   </cols>
   <sheetData>
     <row r="6" spans="7:22" x14ac:dyDescent="0.2">
-      <c r="I6" s="60" t="s">
+      <c r="I6" s="65" t="s">
         <v>7</v>
       </c>
-      <c r="J6" s="60"/>
-      <c r="K6" s="62"/>
-      <c r="L6" s="62"/>
-      <c r="M6" s="62"/>
-      <c r="N6" s="62"/>
+      <c r="J6" s="65"/>
+      <c r="K6" s="66"/>
+      <c r="L6" s="66"/>
+      <c r="M6" s="66"/>
+      <c r="N6" s="66"/>
     </row>
     <row r="7" spans="7:22" x14ac:dyDescent="0.2">
-      <c r="I7" s="62"/>
-      <c r="J7" s="62"/>
-      <c r="K7" s="62"/>
-      <c r="L7" s="62"/>
-      <c r="M7" s="62"/>
-      <c r="N7" s="62"/>
+      <c r="I7" s="66"/>
+      <c r="J7" s="66"/>
+      <c r="K7" s="66"/>
+      <c r="L7" s="66"/>
+      <c r="M7" s="66"/>
+      <c r="N7" s="66"/>
     </row>
     <row r="8" spans="7:22" ht="17" thickBot="1" x14ac:dyDescent="0.25"/>
     <row r="9" spans="7:22" ht="82" customHeight="1" x14ac:dyDescent="0.2">
       <c r="G9" s="1"/>
-      <c r="H9" s="58" t="s">
+      <c r="H9" s="63" t="s">
         <v>8</v>
       </c>
-      <c r="I9" s="59"/>
+      <c r="I9" s="64"/>
       <c r="J9" s="25"/>
-      <c r="K9" s="58" t="s">
+      <c r="K9" s="63" t="s">
         <v>9</v>
       </c>
-      <c r="L9" s="59"/>
+      <c r="L9" s="64"/>
       <c r="M9" s="25"/>
-      <c r="N9" s="58" t="s">
+      <c r="N9" s="63" t="s">
         <v>10</v>
       </c>
-      <c r="O9" s="59"/>
+      <c r="O9" s="64"/>
       <c r="P9" s="25"/>
-      <c r="Q9" s="58" t="s">
+      <c r="Q9" s="63" t="s">
         <v>11</v>
       </c>
-      <c r="R9" s="59"/>
+      <c r="R9" s="64"/>
       <c r="S9" s="25"/>
-      <c r="T9" s="58" t="s">
+      <c r="T9" s="63" t="s">
         <v>79</v>
       </c>
-      <c r="U9" s="59"/>
+      <c r="U9" s="64"/>
       <c r="V9" s="2"/>
     </row>
     <row r="10" spans="7:22" ht="21" x14ac:dyDescent="0.25">
@@ -2473,7 +2481,7 @@
     </row>
     <row r="12" spans="7:22" ht="70" x14ac:dyDescent="0.25">
       <c r="G12" s="45" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
       <c r="H12" s="9">
         <v>1</v>
@@ -2482,7 +2490,7 @@
         <v>17</v>
       </c>
       <c r="J12" s="45" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
       <c r="K12" s="9">
         <v>1</v>
@@ -2491,7 +2499,7 @@
         <v>28</v>
       </c>
       <c r="M12" s="45" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
       <c r="N12" s="9">
         <v>1</v>
@@ -2500,7 +2508,7 @@
         <v>39</v>
       </c>
       <c r="P12" s="45" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
       <c r="Q12" s="9">
         <v>1</v>
@@ -2509,7 +2517,7 @@
         <v>47</v>
       </c>
       <c r="S12" s="45" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
       <c r="T12" s="9">
         <v>1</v>
@@ -2520,7 +2528,7 @@
     </row>
     <row r="13" spans="7:22" ht="70" x14ac:dyDescent="0.25">
       <c r="G13" s="45" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
       <c r="H13" s="9">
         <v>1</v>
@@ -2529,7 +2537,7 @@
         <v>18</v>
       </c>
       <c r="J13" s="45" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
       <c r="K13" s="9">
         <v>1</v>
@@ -2538,7 +2546,7 @@
         <v>29</v>
       </c>
       <c r="M13" s="46" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
       <c r="N13" s="9">
         <v>1</v>
@@ -2547,7 +2555,7 @@
         <v>40</v>
       </c>
       <c r="P13" s="46" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
       <c r="Q13" s="9">
         <v>1</v>
@@ -2556,7 +2564,7 @@
         <v>48</v>
       </c>
       <c r="S13" s="45" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
       <c r="T13" s="9">
         <v>1</v>
@@ -2567,7 +2575,7 @@
     </row>
     <row r="14" spans="7:22" ht="70" x14ac:dyDescent="0.25">
       <c r="G14" s="46" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="H14" s="9">
         <v>1</v>
@@ -2576,7 +2584,7 @@
         <v>25</v>
       </c>
       <c r="J14" s="45" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
       <c r="K14" s="9">
         <v>1</v>
@@ -2585,7 +2593,7 @@
         <v>36</v>
       </c>
       <c r="M14" s="45" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
       <c r="N14" s="9">
         <v>1</v>
@@ -2594,7 +2602,7 @@
         <v>38</v>
       </c>
       <c r="P14" s="45" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
       <c r="Q14" s="9">
         <v>1</v>
@@ -2603,7 +2611,7 @@
         <v>55</v>
       </c>
       <c r="S14" s="45" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
       <c r="T14" s="9">
         <v>1</v>
@@ -2614,7 +2622,7 @@
     </row>
     <row r="15" spans="7:22" ht="70" x14ac:dyDescent="0.25">
       <c r="G15" s="46" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
       <c r="H15" s="9">
         <v>1</v>
@@ -2623,7 +2631,7 @@
         <v>19</v>
       </c>
       <c r="J15" s="45" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
       <c r="K15" s="9">
         <v>1</v>
@@ -2632,7 +2640,7 @@
         <v>30</v>
       </c>
       <c r="M15" s="46" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
       <c r="N15" s="9">
         <v>1</v>
@@ -2641,7 +2649,7 @@
         <v>41</v>
       </c>
       <c r="P15" s="46" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
       <c r="Q15" s="9">
         <v>1</v>
@@ -2650,7 +2658,7 @@
         <v>49</v>
       </c>
       <c r="S15" s="45" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
       <c r="T15" s="9">
         <v>1</v>
@@ -2661,7 +2669,7 @@
     </row>
     <row r="16" spans="7:22" ht="70" x14ac:dyDescent="0.25">
       <c r="G16" s="46" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
       <c r="H16" s="9">
         <v>1</v>
@@ -2670,7 +2678,7 @@
         <v>20</v>
       </c>
       <c r="J16" s="46" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
       <c r="K16" s="9">
         <v>1</v>
@@ -2679,7 +2687,7 @@
         <v>31</v>
       </c>
       <c r="M16" s="46" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
       <c r="N16" s="9">
         <v>1</v>
@@ -2688,7 +2696,7 @@
         <v>42</v>
       </c>
       <c r="P16" s="46" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
       <c r="Q16" s="9">
         <v>1</v>
@@ -2697,7 +2705,7 @@
         <v>50</v>
       </c>
       <c r="S16" s="45" t="s">
-        <v>145</v>
+        <v>144</v>
       </c>
       <c r="T16" s="9">
         <v>1</v>
@@ -2708,7 +2716,7 @@
     </row>
     <row r="17" spans="6:22" ht="70" x14ac:dyDescent="0.25">
       <c r="G17" s="46" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
       <c r="H17" s="9">
         <v>1</v>
@@ -2717,7 +2725,7 @@
         <v>21</v>
       </c>
       <c r="J17" s="46" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
       <c r="K17" s="9">
         <v>1</v>
@@ -2726,7 +2734,7 @@
         <v>32</v>
       </c>
       <c r="M17" s="46" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
       <c r="N17" s="9">
         <v>1</v>
@@ -2735,7 +2743,7 @@
         <v>43</v>
       </c>
       <c r="P17" s="46" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
       <c r="Q17" s="9">
         <v>1</v>
@@ -2744,7 +2752,7 @@
         <v>51</v>
       </c>
       <c r="S17" s="45" t="s">
-        <v>146</v>
+        <v>145</v>
       </c>
       <c r="T17" s="9">
         <v>1</v>
@@ -2755,7 +2763,7 @@
     </row>
     <row r="18" spans="6:22" ht="70" x14ac:dyDescent="0.25">
       <c r="G18" s="46" t="s">
-        <v>139</v>
+        <v>138</v>
       </c>
       <c r="H18" s="9">
         <v>1</v>
@@ -2764,7 +2772,7 @@
         <v>22</v>
       </c>
       <c r="J18" s="46" t="s">
-        <v>139</v>
+        <v>138</v>
       </c>
       <c r="K18" s="9">
         <v>1</v>
@@ -2773,7 +2781,7 @@
         <v>33</v>
       </c>
       <c r="M18" s="46" t="s">
-        <v>139</v>
+        <v>138</v>
       </c>
       <c r="N18" s="9">
         <v>1</v>
@@ -2782,7 +2790,7 @@
         <v>44</v>
       </c>
       <c r="P18" s="46" t="s">
-        <v>139</v>
+        <v>138</v>
       </c>
       <c r="Q18" s="9">
         <v>1</v>
@@ -2791,7 +2799,7 @@
         <v>52</v>
       </c>
       <c r="S18" s="45" t="s">
-        <v>147</v>
+        <v>146</v>
       </c>
       <c r="T18" s="9">
         <v>1</v>
@@ -2802,7 +2810,7 @@
     </row>
     <row r="19" spans="6:22" ht="70" x14ac:dyDescent="0.25">
       <c r="G19" s="47" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
       <c r="H19" s="33" t="s">
         <v>3</v>
@@ -2811,7 +2819,7 @@
         <v>23</v>
       </c>
       <c r="J19" s="46" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
       <c r="K19" s="9">
         <v>1</v>
@@ -2820,7 +2828,7 @@
         <v>34</v>
       </c>
       <c r="M19" s="46" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
       <c r="N19" s="9">
         <v>1</v>
@@ -2829,7 +2837,7 @@
         <v>45</v>
       </c>
       <c r="P19" s="46" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
       <c r="Q19" s="9">
         <v>1</v>
@@ -2838,7 +2846,7 @@
         <v>53</v>
       </c>
       <c r="S19" s="48" t="s">
-        <v>148</v>
+        <v>147</v>
       </c>
       <c r="T19" s="31" t="s">
         <v>3</v>
@@ -2849,7 +2857,7 @@
     </row>
     <row r="20" spans="6:22" ht="71" thickBot="1" x14ac:dyDescent="0.3">
       <c r="G20" s="47" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
       <c r="H20" s="35" t="s">
         <v>3</v>
@@ -2858,7 +2866,7 @@
         <v>24</v>
       </c>
       <c r="J20" s="47" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
       <c r="K20" s="35" t="s">
         <v>3</v>
@@ -2867,7 +2875,7 @@
         <v>35</v>
       </c>
       <c r="M20" s="47" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
       <c r="N20" s="35" t="s">
         <v>3</v>
@@ -2876,7 +2884,7 @@
         <v>46</v>
       </c>
       <c r="P20" s="47" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
       <c r="Q20" s="35" t="s">
         <v>3</v>
@@ -2885,7 +2893,7 @@
         <v>54</v>
       </c>
       <c r="S20" s="49" t="s">
-        <v>149</v>
+        <v>148</v>
       </c>
       <c r="T20" s="31" t="s">
         <v>3</v>
@@ -2896,7 +2904,7 @@
     </row>
     <row r="21" spans="6:22" ht="92" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="G21" s="39" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
       <c r="H21" s="14"/>
       <c r="I21" s="40">
@@ -2924,9 +2932,9 @@
       </c>
     </row>
     <row r="22" spans="6:22" ht="25" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="F22" s="64"/>
+      <c r="F22" s="54"/>
       <c r="G22" s="40" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
       <c r="H22" s="14"/>
       <c r="I22" s="40">
@@ -2950,11 +2958,11 @@
       <c r="V22" s="2"/>
     </row>
     <row r="23" spans="6:22" ht="25" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="F23" s="64"/>
+      <c r="F23" s="54"/>
       <c r="G23" s="40" t="s">
-        <v>152</v>
-      </c>
-      <c r="H23" s="65"/>
+        <v>151</v>
+      </c>
+      <c r="H23" s="55"/>
       <c r="I23" s="40">
         <v>0.95</v>
       </c>
@@ -2972,7 +2980,7 @@
       <c r="R23" s="43">
         <v>1</v>
       </c>
-      <c r="S23" s="65"/>
+      <c r="S23" s="55"/>
       <c r="U23" s="43">
         <v>1</v>
       </c>
@@ -2980,12 +2988,12 @@
     </row>
     <row r="24" spans="6:22" x14ac:dyDescent="0.2">
       <c r="L24" s="23"/>
-      <c r="N24" s="66"/>
-      <c r="O24" s="66"/>
-      <c r="P24" s="66"/>
-      <c r="Q24" s="66"/>
-      <c r="R24" s="66"/>
-      <c r="T24" s="66"/>
+      <c r="N24" s="56"/>
+      <c r="O24" s="56"/>
+      <c r="P24" s="56"/>
+      <c r="Q24" s="56"/>
+      <c r="R24" s="56"/>
+      <c r="T24" s="56"/>
     </row>
     <row r="25" spans="6:22" ht="34" x14ac:dyDescent="0.2">
       <c r="G25" s="12"/>
@@ -2996,82 +3004,82 @@
       <c r="J25" s="13"/>
     </row>
     <row r="26" spans="6:22" ht="49" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="G26" s="54"/>
-      <c r="H26" s="54"/>
-      <c r="I26" s="54"/>
+      <c r="G26" s="72"/>
+      <c r="H26" s="72"/>
+      <c r="I26" s="72"/>
       <c r="L26" t="s">
-        <v>150</v>
+        <v>149</v>
       </c>
     </row>
     <row r="30" spans="6:22" ht="16" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="I30" s="60"/>
-      <c r="J30" s="60"/>
-      <c r="K30" s="60"/>
-      <c r="L30" s="60"/>
-      <c r="M30" s="60"/>
-      <c r="N30" s="60"/>
+      <c r="I30" s="65"/>
+      <c r="J30" s="65"/>
+      <c r="K30" s="65"/>
+      <c r="L30" s="65"/>
+      <c r="M30" s="65"/>
+      <c r="N30" s="65"/>
     </row>
     <row r="31" spans="6:22" ht="17" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="I31" s="60"/>
-      <c r="J31" s="60"/>
-      <c r="K31" s="60"/>
-      <c r="L31" s="60"/>
-      <c r="M31" s="60"/>
-      <c r="N31" s="60"/>
+      <c r="I31" s="65"/>
+      <c r="J31" s="65"/>
+      <c r="K31" s="65"/>
+      <c r="L31" s="65"/>
+      <c r="M31" s="65"/>
+      <c r="N31" s="65"/>
     </row>
     <row r="32" spans="6:22" ht="25" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="G32" s="55" t="s">
+      <c r="G32" s="68" t="s">
         <v>13</v>
       </c>
-      <c r="H32" s="56"/>
-      <c r="I32" s="57"/>
-      <c r="J32" s="55" t="s">
+      <c r="H32" s="69"/>
+      <c r="I32" s="70"/>
+      <c r="J32" s="68" t="s">
         <v>14</v>
       </c>
-      <c r="K32" s="56"/>
-      <c r="L32" s="57"/>
-      <c r="M32" s="55" t="s">
+      <c r="K32" s="69"/>
+      <c r="L32" s="70"/>
+      <c r="M32" s="68" t="s">
+        <v>126</v>
+      </c>
+      <c r="N32" s="69"/>
+      <c r="O32" s="70"/>
+      <c r="P32" s="68" t="s">
         <v>127</v>
       </c>
-      <c r="N32" s="56"/>
-      <c r="O32" s="57"/>
-      <c r="P32" s="55" t="s">
+      <c r="Q32" s="69"/>
+      <c r="R32" s="70"/>
+      <c r="S32" s="68" t="s">
         <v>128</v>
       </c>
-      <c r="Q32" s="56"/>
-      <c r="R32" s="57"/>
-      <c r="S32" s="55" t="s">
-        <v>129</v>
-      </c>
-      <c r="T32" s="56"/>
-      <c r="U32" s="57"/>
+      <c r="T32" s="69"/>
+      <c r="U32" s="70"/>
     </row>
     <row r="33" spans="7:21" ht="50" customHeight="1" x14ac:dyDescent="0.2">
       <c r="G33" s="1"/>
-      <c r="H33" s="58" t="s">
+      <c r="H33" s="63" t="s">
         <v>78</v>
       </c>
-      <c r="I33" s="63"/>
+      <c r="I33" s="71"/>
       <c r="J33" s="1"/>
-      <c r="K33" s="58" t="s">
+      <c r="K33" s="63" t="s">
         <v>78</v>
       </c>
-      <c r="L33" s="59"/>
+      <c r="L33" s="64"/>
       <c r="M33" s="1"/>
-      <c r="N33" s="58" t="s">
+      <c r="N33" s="63" t="s">
         <v>78</v>
       </c>
-      <c r="O33" s="59"/>
+      <c r="O33" s="64"/>
       <c r="P33" s="1"/>
-      <c r="Q33" s="58" t="s">
+      <c r="Q33" s="63" t="s">
         <v>78</v>
       </c>
-      <c r="R33" s="59"/>
+      <c r="R33" s="64"/>
       <c r="S33" s="1"/>
-      <c r="T33" s="58" t="s">
+      <c r="T33" s="63" t="s">
         <v>78</v>
       </c>
-      <c r="U33" s="59"/>
+      <c r="U33" s="64"/>
     </row>
     <row r="34" spans="7:21" ht="21" x14ac:dyDescent="0.25">
       <c r="G34" s="2"/>
@@ -3159,7 +3167,7 @@
     </row>
     <row r="36" spans="7:21" ht="24" x14ac:dyDescent="0.3">
       <c r="G36" s="4" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="H36" s="9">
         <v>1</v>
@@ -3168,7 +3176,7 @@
         <v>67</v>
       </c>
       <c r="J36" s="4" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="K36" s="9">
         <v>1</v>
@@ -3177,7 +3185,7 @@
         <v>81</v>
       </c>
       <c r="M36" s="4" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="N36" s="9">
         <v>1</v>
@@ -3186,7 +3194,7 @@
         <v>92</v>
       </c>
       <c r="P36" s="30" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="Q36" s="31" t="s">
         <v>96</v>
@@ -3195,7 +3203,7 @@
         <v>97</v>
       </c>
       <c r="S36" s="30" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="T36" s="31" t="s">
         <v>102</v>
@@ -3206,7 +3214,7 @@
     </row>
     <row r="37" spans="7:21" ht="24" x14ac:dyDescent="0.3">
       <c r="G37" s="4" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="H37" s="9">
         <v>1</v>
@@ -3215,7 +3223,7 @@
         <v>68</v>
       </c>
       <c r="J37" s="4" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="K37" s="9">
         <v>1</v>
@@ -3224,7 +3232,7 @@
         <v>82</v>
       </c>
       <c r="M37" s="30" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="N37" s="31" t="s">
         <v>106</v>
@@ -3233,7 +3241,7 @@
         <v>93</v>
       </c>
       <c r="P37" s="30" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="Q37" s="31" t="s">
         <v>98</v>
@@ -3242,7 +3250,7 @@
         <v>99</v>
       </c>
       <c r="S37" s="30" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="T37" s="31" t="s">
         <v>102</v>
@@ -3253,7 +3261,7 @@
     </row>
     <row r="38" spans="7:21" ht="24" x14ac:dyDescent="0.3">
       <c r="G38" s="4" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="H38" s="9">
         <v>1</v>
@@ -3262,7 +3270,7 @@
         <v>69</v>
       </c>
       <c r="J38" s="30" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="K38" s="31" t="s">
         <v>73</v>
@@ -3271,16 +3279,16 @@
         <v>83</v>
       </c>
       <c r="M38" s="30" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="N38" s="31" t="s">
         <v>73</v>
       </c>
       <c r="O38" s="32" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="P38" s="30" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="Q38" s="31" t="s">
         <v>98</v>
@@ -3289,18 +3297,18 @@
         <v>100</v>
       </c>
       <c r="S38" s="30" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="T38" s="31" t="s">
-        <v>98</v>
+        <v>170</v>
       </c>
       <c r="U38" s="32" t="s">
-        <v>100</v>
+        <v>109</v>
       </c>
     </row>
     <row r="39" spans="7:21" ht="24" x14ac:dyDescent="0.3">
       <c r="G39" s="4" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="H39" s="9">
         <v>1</v>
@@ -3309,7 +3317,7 @@
         <v>70</v>
       </c>
       <c r="J39" s="30" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="K39" s="31" t="s">
         <v>73</v>
@@ -3318,16 +3326,16 @@
         <v>84</v>
       </c>
       <c r="M39" s="50" t="s">
+        <v>120</v>
+      </c>
+      <c r="N39" s="51">
+        <v>1</v>
+      </c>
+      <c r="O39" s="52" t="s">
         <v>121</v>
       </c>
-      <c r="N39" s="51">
-        <v>1</v>
-      </c>
-      <c r="O39" s="52" t="s">
-        <v>122</v>
-      </c>
       <c r="P39" s="30" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="Q39" s="31" t="s">
         <v>98</v>
@@ -3336,18 +3344,18 @@
         <v>101</v>
       </c>
       <c r="S39" s="30" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="T39" s="31" t="s">
-        <v>109</v>
+        <v>170</v>
       </c>
       <c r="U39" s="32" t="s">
-        <v>110</v>
+        <v>171</v>
       </c>
     </row>
     <row r="40" spans="7:21" ht="24" x14ac:dyDescent="0.3">
       <c r="G40" s="4" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
       <c r="H40" s="9">
         <v>1</v>
@@ -3356,7 +3364,7 @@
         <v>71</v>
       </c>
       <c r="J40" s="30" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
       <c r="K40" s="31" t="s">
         <v>3</v>
@@ -3365,16 +3373,16 @@
         <v>85</v>
       </c>
       <c r="M40" s="50" t="s">
+        <v>122</v>
+      </c>
+      <c r="N40" s="51">
+        <v>1</v>
+      </c>
+      <c r="O40" s="52" t="s">
         <v>123</v>
       </c>
-      <c r="N40" s="51">
-        <v>1</v>
-      </c>
-      <c r="O40" s="52" t="s">
-        <v>124</v>
-      </c>
       <c r="P40" s="30" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
       <c r="Q40" s="31" t="s">
         <v>102</v>
@@ -3383,18 +3391,18 @@
         <v>103</v>
       </c>
       <c r="S40" s="30" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
       <c r="T40" s="31" t="s">
-        <v>102</v>
+        <v>173</v>
       </c>
       <c r="U40" s="32" t="s">
-        <v>103</v>
+        <v>172</v>
       </c>
     </row>
     <row r="41" spans="7:21" ht="24" x14ac:dyDescent="0.3">
       <c r="G41" s="30" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
       <c r="H41" s="31" t="s">
         <v>73</v>
@@ -3403,7 +3411,7 @@
         <v>72</v>
       </c>
       <c r="J41" s="30" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
       <c r="K41" s="31" t="s">
         <v>75</v>
@@ -3412,28 +3420,28 @@
         <v>86</v>
       </c>
       <c r="M41" s="50" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
       <c r="N41" s="53" t="s">
         <v>3</v>
       </c>
       <c r="O41" s="52" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
       <c r="P41" s="4" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
       <c r="Q41" s="9"/>
       <c r="R41" s="5"/>
       <c r="S41" s="4" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
       <c r="T41" s="9"/>
       <c r="U41" s="5"/>
     </row>
     <row r="42" spans="7:21" ht="24" x14ac:dyDescent="0.3">
       <c r="G42" s="30" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="H42" s="31" t="s">
         <v>73</v>
@@ -3442,7 +3450,7 @@
         <v>74</v>
       </c>
       <c r="J42" s="30" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="K42" s="31" t="s">
         <v>75</v>
@@ -3451,7 +3459,7 @@
         <v>87</v>
       </c>
       <c r="M42" s="30" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="N42" s="31" t="s">
         <v>73</v>
@@ -3460,19 +3468,19 @@
         <v>94</v>
       </c>
       <c r="P42" s="4" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="Q42" s="9"/>
       <c r="R42" s="5"/>
       <c r="S42" s="4" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="T42" s="9"/>
       <c r="U42" s="5"/>
     </row>
     <row r="43" spans="7:21" ht="24" x14ac:dyDescent="0.3">
       <c r="G43" s="30" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
       <c r="H43" s="33" t="s">
         <v>75</v>
@@ -3481,7 +3489,7 @@
         <v>76</v>
       </c>
       <c r="J43" s="30" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
       <c r="K43" s="33" t="s">
         <v>75</v>
@@ -3490,7 +3498,7 @@
         <v>88</v>
       </c>
       <c r="M43" s="30" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
       <c r="N43" s="31" t="s">
         <v>104</v>
@@ -3499,19 +3507,19 @@
         <v>105</v>
       </c>
       <c r="P43" s="4" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
       <c r="Q43" s="11"/>
       <c r="R43" s="5"/>
       <c r="S43" s="4" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
       <c r="T43" s="11"/>
       <c r="U43" s="5"/>
     </row>
     <row r="44" spans="7:21" ht="25" thickBot="1" x14ac:dyDescent="0.35">
       <c r="G44" s="34" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
       <c r="H44" s="35" t="s">
         <v>12</v>
@@ -3520,7 +3528,7 @@
         <v>77</v>
       </c>
       <c r="J44" s="34" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
       <c r="K44" s="35" t="s">
         <v>90</v>
@@ -3529,50 +3537,50 @@
         <v>89</v>
       </c>
       <c r="M44" s="4" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
       <c r="N44" s="9"/>
       <c r="O44" s="5"/>
       <c r="P44" s="6" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
       <c r="Q44" s="10"/>
       <c r="R44" s="7"/>
       <c r="S44" s="6" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
       <c r="T44" s="10"/>
       <c r="U44" s="7"/>
     </row>
     <row r="45" spans="7:21" ht="25" thickBot="1" x14ac:dyDescent="0.35">
       <c r="G45" s="44" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
       <c r="H45" s="14"/>
       <c r="I45" s="42">
         <v>0.69</v>
       </c>
       <c r="J45" s="44" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
       <c r="K45" s="14"/>
       <c r="L45" s="42">
         <v>0.94</v>
       </c>
       <c r="M45" s="4" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="N45" s="9"/>
       <c r="O45" s="5"/>
       <c r="P45" s="44" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
       <c r="Q45" s="14"/>
       <c r="R45" s="42">
         <v>0.82</v>
       </c>
       <c r="S45" s="44" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
       <c r="T45" s="14"/>
       <c r="U45" s="42">
@@ -3581,7 +3589,7 @@
     </row>
     <row r="46" spans="7:21" ht="25" thickBot="1" x14ac:dyDescent="0.35">
       <c r="G46" s="30" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
       <c r="I46" s="42">
         <v>0.71</v>
@@ -3590,12 +3598,12 @@
         <v>0.99</v>
       </c>
       <c r="M46" s="4" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
       <c r="N46" s="11"/>
       <c r="O46" s="5"/>
-      <c r="P46" s="70" t="s">
-        <v>151</v>
+      <c r="P46" s="59" t="s">
+        <v>150</v>
       </c>
       <c r="Q46" s="14"/>
       <c r="R46" s="42">
@@ -3607,51 +3615,51 @@
       </c>
     </row>
     <row r="47" spans="7:21" ht="25" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="G47" s="67" t="s">
-        <v>152</v>
+      <c r="G47" s="57" t="s">
+        <v>151</v>
       </c>
       <c r="H47" s="14"/>
       <c r="I47" s="42">
         <v>0.98</v>
       </c>
-      <c r="J47" s="68"/>
+      <c r="J47" s="58"/>
       <c r="K47" s="14"/>
       <c r="L47" s="42">
         <v>1</v>
       </c>
       <c r="M47" s="6" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
       <c r="N47" s="10"/>
       <c r="O47" s="7"/>
-      <c r="P47" s="69" t="s">
-        <v>152</v>
+      <c r="P47" s="4" t="s">
+        <v>151</v>
       </c>
       <c r="Q47" s="14"/>
       <c r="R47" s="42">
         <v>1</v>
       </c>
-      <c r="S47" s="68"/>
+      <c r="S47" s="58"/>
       <c r="U47" s="42">
         <v>0.33</v>
       </c>
     </row>
     <row r="48" spans="7:21" ht="23" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="J48" s="66"/>
+      <c r="J48" s="56"/>
       <c r="M48" s="44" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
       <c r="N48" s="14"/>
       <c r="O48" s="42">
         <v>0.94</v>
       </c>
-      <c r="P48" s="68"/>
-      <c r="S48" s="66"/>
-      <c r="T48" s="66"/>
+      <c r="P48" s="58"/>
+      <c r="S48" s="56"/>
+      <c r="T48" s="56"/>
     </row>
     <row r="49" spans="9:16" ht="23" thickBot="1" x14ac:dyDescent="0.3">
       <c r="M49" s="44" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
       <c r="O49" s="42">
         <v>0.96</v>
@@ -3659,7 +3667,7 @@
     </row>
     <row r="50" spans="9:16" ht="23" thickBot="1" x14ac:dyDescent="0.3">
       <c r="M50" s="44" t="s">
-        <v>152</v>
+        <v>151</v>
       </c>
       <c r="N50" s="14"/>
       <c r="O50" s="42">
@@ -3667,34 +3675,34 @@
       </c>
     </row>
     <row r="51" spans="9:16" x14ac:dyDescent="0.2">
-      <c r="M51" s="66"/>
+      <c r="M51" s="56"/>
     </row>
     <row r="55" spans="9:16" x14ac:dyDescent="0.2">
-      <c r="I55" s="60"/>
-      <c r="J55" s="60"/>
-      <c r="K55" s="62"/>
-      <c r="L55" s="62"/>
-      <c r="M55" s="62"/>
-      <c r="N55" s="62"/>
+      <c r="I55" s="65"/>
+      <c r="J55" s="65"/>
+      <c r="K55" s="66"/>
+      <c r="L55" s="66"/>
+      <c r="M55" s="66"/>
+      <c r="N55" s="66"/>
     </row>
     <row r="56" spans="9:16" x14ac:dyDescent="0.2">
-      <c r="I56" s="62"/>
-      <c r="J56" s="62"/>
-      <c r="K56" s="62"/>
-      <c r="L56" s="62"/>
-      <c r="M56" s="62"/>
-      <c r="N56" s="62"/>
+      <c r="I56" s="66"/>
+      <c r="J56" s="66"/>
+      <c r="K56" s="66"/>
+      <c r="L56" s="66"/>
+      <c r="M56" s="66"/>
+      <c r="N56" s="66"/>
     </row>
     <row r="57" spans="9:16" ht="24" x14ac:dyDescent="0.3">
       <c r="J57" s="26"/>
     </row>
     <row r="58" spans="9:16" ht="58" customHeight="1" x14ac:dyDescent="0.2">
       <c r="J58" s="17"/>
-      <c r="K58" s="61"/>
-      <c r="L58" s="62"/>
+      <c r="K58" s="67"/>
+      <c r="L58" s="66"/>
       <c r="M58" s="17"/>
-      <c r="N58" s="61"/>
-      <c r="O58" s="62"/>
+      <c r="N58" s="67"/>
+      <c r="O58" s="66"/>
       <c r="P58" s="17"/>
     </row>
     <row r="59" spans="9:16" ht="21" x14ac:dyDescent="0.25">
@@ -3736,7 +3744,7 @@
     <row r="63" spans="9:16" ht="22" thickBot="1" x14ac:dyDescent="0.3">
       <c r="J63" s="20"/>
       <c r="K63" s="21"/>
-      <c r="L63" s="71"/>
+      <c r="L63" s="60"/>
       <c r="M63" s="20"/>
       <c r="N63" s="21"/>
       <c r="O63" s="20"/>
@@ -3745,9 +3753,9 @@
     <row r="64" spans="9:16" ht="21" x14ac:dyDescent="0.25">
       <c r="J64" s="20"/>
       <c r="K64" s="21"/>
-      <c r="L64" s="73"/>
-      <c r="M64" s="72" t="s">
-        <v>153</v>
+      <c r="L64" s="62"/>
+      <c r="M64" s="61" t="s">
+        <v>152</v>
       </c>
       <c r="N64" s="21"/>
       <c r="O64" s="20"/>
@@ -3758,7 +3766,7 @@
       <c r="K65" s="21"/>
       <c r="L65" s="11"/>
       <c r="M65" s="5" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
       <c r="N65" s="21"/>
       <c r="O65" s="20"/>
@@ -3771,7 +3779,7 @@
         <v>0</v>
       </c>
       <c r="M66" s="5" t="s">
-        <v>161</v>
+        <v>160</v>
       </c>
       <c r="N66" s="21"/>
       <c r="O66" s="20"/>
@@ -3781,10 +3789,10 @@
       <c r="J67" s="20"/>
       <c r="K67" s="21"/>
       <c r="L67" s="11" t="s">
-        <v>155</v>
+        <v>154</v>
       </c>
       <c r="M67" s="5" t="s">
-        <v>162</v>
+        <v>161</v>
       </c>
       <c r="N67" s="21"/>
       <c r="O67" s="20"/>
@@ -3794,10 +3802,10 @@
       <c r="J68" s="20"/>
       <c r="K68" s="21"/>
       <c r="L68" s="11" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
       <c r="M68" s="5" t="s">
-        <v>163</v>
+        <v>162</v>
       </c>
       <c r="N68" s="21"/>
       <c r="O68" s="20"/>
@@ -3807,10 +3815,10 @@
       <c r="J69" s="20"/>
       <c r="K69" s="20"/>
       <c r="L69" s="11" t="s">
-        <v>157</v>
+        <v>156</v>
       </c>
       <c r="M69" s="5" t="s">
-        <v>164</v>
+        <v>163</v>
       </c>
       <c r="N69" s="20"/>
       <c r="O69" s="20"/>
@@ -3820,10 +3828,10 @@
       <c r="J70" s="22"/>
       <c r="K70" s="17"/>
       <c r="L70" s="11" t="s">
-        <v>158</v>
+        <v>157</v>
       </c>
       <c r="M70" s="5" t="s">
-        <v>165</v>
+        <v>164</v>
       </c>
       <c r="N70" s="17"/>
       <c r="O70" s="22"/>
@@ -3831,73 +3839,73 @@
     </row>
     <row r="71" spans="9:16" ht="21" x14ac:dyDescent="0.25">
       <c r="L71" s="11" t="s">
-        <v>159</v>
+        <v>158</v>
       </c>
       <c r="M71" s="5" t="s">
-        <v>166</v>
+        <v>165</v>
       </c>
     </row>
     <row r="72" spans="9:16" ht="21" x14ac:dyDescent="0.25">
       <c r="L72" s="11" t="s">
-        <v>160</v>
+        <v>159</v>
       </c>
       <c r="M72" s="5" t="s">
-        <v>167</v>
+        <v>166</v>
       </c>
     </row>
     <row r="73" spans="9:16" ht="21" x14ac:dyDescent="0.25">
       <c r="L73" s="11" t="s">
+        <v>167</v>
+      </c>
+      <c r="M73" s="5" t="s">
         <v>168</v>
-      </c>
-      <c r="M73" s="5" t="s">
-        <v>169</v>
       </c>
     </row>
     <row r="74" spans="9:16" ht="21" x14ac:dyDescent="0.25">
       <c r="L74" s="11" t="s">
-        <v>152</v>
+        <v>151</v>
       </c>
       <c r="M74" s="5" t="s">
-        <v>170</v>
+        <v>169</v>
       </c>
     </row>
     <row r="75" spans="9:16" ht="22" thickBot="1" x14ac:dyDescent="0.3">
       <c r="L75" s="11" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
       <c r="M75" s="7" t="s">
-        <v>169</v>
+        <v>168</v>
       </c>
     </row>
     <row r="76" spans="9:16" x14ac:dyDescent="0.2">
-      <c r="L76" s="66"/>
+      <c r="L76" s="56"/>
     </row>
     <row r="77" spans="9:16" x14ac:dyDescent="0.2">
-      <c r="I77" s="60"/>
-      <c r="J77" s="60"/>
-      <c r="K77" s="62"/>
-      <c r="L77" s="62"/>
-      <c r="M77" s="62"/>
-      <c r="N77" s="62"/>
+      <c r="I77" s="65"/>
+      <c r="J77" s="65"/>
+      <c r="K77" s="66"/>
+      <c r="L77" s="66"/>
+      <c r="M77" s="66"/>
+      <c r="N77" s="66"/>
     </row>
     <row r="78" spans="9:16" x14ac:dyDescent="0.2">
-      <c r="I78" s="62"/>
-      <c r="J78" s="62"/>
-      <c r="K78" s="62"/>
-      <c r="L78" s="62"/>
-      <c r="M78" s="62"/>
-      <c r="N78" s="62"/>
+      <c r="I78" s="66"/>
+      <c r="J78" s="66"/>
+      <c r="K78" s="66"/>
+      <c r="L78" s="66"/>
+      <c r="M78" s="66"/>
+      <c r="N78" s="66"/>
     </row>
     <row r="79" spans="9:16" ht="24" x14ac:dyDescent="0.3">
       <c r="J79" s="26"/>
     </row>
     <row r="80" spans="9:16" ht="59" customHeight="1" x14ac:dyDescent="0.2">
       <c r="J80" s="17"/>
-      <c r="K80" s="61"/>
-      <c r="L80" s="62"/>
+      <c r="K80" s="67"/>
+      <c r="L80" s="66"/>
       <c r="M80" s="17"/>
-      <c r="N80" s="61"/>
-      <c r="O80" s="62"/>
+      <c r="N80" s="67"/>
+      <c r="O80" s="66"/>
       <c r="P80" s="17"/>
     </row>
     <row r="81" spans="10:18" ht="21" x14ac:dyDescent="0.25">
@@ -4046,12 +4054,14 @@
     <row r="104" ht="62" customHeight="1" x14ac:dyDescent="0.2"/>
   </sheetData>
   <mergeCells count="24">
-    <mergeCell ref="T9:U9"/>
-    <mergeCell ref="I6:N7"/>
-    <mergeCell ref="Q9:R9"/>
-    <mergeCell ref="H9:I9"/>
-    <mergeCell ref="K9:L9"/>
-    <mergeCell ref="N9:O9"/>
+    <mergeCell ref="G26:I26"/>
+    <mergeCell ref="G32:I32"/>
+    <mergeCell ref="P32:R32"/>
+    <mergeCell ref="Q33:R33"/>
+    <mergeCell ref="S32:U32"/>
+    <mergeCell ref="T33:U33"/>
+    <mergeCell ref="N33:O33"/>
+    <mergeCell ref="I30:N31"/>
     <mergeCell ref="K80:L80"/>
     <mergeCell ref="N80:O80"/>
     <mergeCell ref="J32:L32"/>
@@ -4062,14 +4072,12 @@
     <mergeCell ref="N58:O58"/>
     <mergeCell ref="I77:N78"/>
     <mergeCell ref="H33:I33"/>
-    <mergeCell ref="G26:I26"/>
-    <mergeCell ref="G32:I32"/>
-    <mergeCell ref="P32:R32"/>
-    <mergeCell ref="Q33:R33"/>
-    <mergeCell ref="S32:U32"/>
-    <mergeCell ref="T33:U33"/>
-    <mergeCell ref="N33:O33"/>
-    <mergeCell ref="I30:N31"/>
+    <mergeCell ref="T9:U9"/>
+    <mergeCell ref="I6:N7"/>
+    <mergeCell ref="Q9:R9"/>
+    <mergeCell ref="H9:I9"/>
+    <mergeCell ref="K9:L9"/>
+    <mergeCell ref="N9:O9"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <drawing r:id="rId1"/>

</xml_diff>